<commit_message>
added most of the Modern Workplace Assessment sheets
added most of the Modern Workplace Assessment sheets
</commit_message>
<xml_diff>
--- a/Assessments/Exam-Msft-MS-101-Self-Assessment-Build5Nines.xlsx
+++ b/Assessments/Exam-Msft-MS-101-Self-Assessment-Build5Nines.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Documents/GitHub/exam-assessments/Assessments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thecloud42ie-my.sharepoint.com/personal/rolf_thecloud42_com/Documents/Customer Projects/TheCloud 42 - Own Courses/done/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF7ED99-34C9-604C-B3B7-2CAB57FB4A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{D5EA79E3-3B76-4DB5-93B0-04371FEDDF8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A1604223-BF37-4546-9766-1CCAFB99DBFA}"/>
   <bookViews>
-    <workbookView xWindow="38480" yWindow="7000" windowWidth="26320" windowHeight="18460" xr2:uid="{C935EA29-66AB-47BC-AD6E-3C33C43244A1}"/>
+    <workbookView xWindow="0" yWindow="3030" windowWidth="33720" windowHeight="19365" xr2:uid="{C935EA29-66AB-47BC-AD6E-3C33C43244A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessment Overview" sheetId="3" r:id="rId1"/>
-    <sheet name="MS-101" sheetId="1" r:id="rId2"/>
+    <sheet name="Self Assessment" sheetId="1" r:id="rId2"/>
     <sheet name="Other Values" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -289,9 +289,6 @@
     <t>No Idea</t>
   </si>
   <si>
-    <t>Self Assessment last updated November 15, 2019</t>
-  </si>
-  <si>
     <t>Keep in mind that all exam Objective Domain info/text is copyright by Microsoft.</t>
   </si>
   <si>
@@ -367,9 +364,6 @@
     <t>Exam MS-101: Microsoft 365 Mobility and Security</t>
   </si>
   <si>
-    <t>https://docs.microsoft.com/learn/certifications/exams/md-101</t>
-  </si>
-  <si>
     <t>Objective Domain</t>
   </si>
   <si>
@@ -386,6 +380,12 @@
   </si>
   <si>
     <t>https://TheCloud42.com</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/learn/certifications/exams/ms-101</t>
+  </si>
+  <si>
+    <t>Self Assessment last updated April 28, 2020</t>
   </si>
 </sst>
 </file>
@@ -1471,187 +1471,187 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="77.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="22" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="3"/>
+    <col min="3" max="3" width="18.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="str">
-        <f>'MS-101'!A2</f>
+        <f>'Self Assessment'!A2</f>
         <v>Implement modern device services (30-35%)</v>
       </c>
       <c r="B16" s="13">
-        <f>'MS-101'!D2</f>
+        <f>'Self Assessment'!D2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="str">
-        <f>'MS-101'!A27</f>
+        <f>'Self Assessment'!A27</f>
         <v>Implement Microsoft 365 security and threat management (30-35%)</v>
       </c>
       <c r="B17" s="13">
-        <f>'MS-101'!D27</f>
+        <f>'Self Assessment'!D27</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="str">
-        <f>'MS-101'!A52</f>
+        <f>'Self Assessment'!A52</f>
         <v>Manage Microsoft 365 governance and compliance (35-40%)</v>
       </c>
       <c r="B18" s="13">
-        <f>'MS-101'!D52</f>
+        <f>'Self Assessment'!D52</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A19" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="11">
         <f>SUM(B16:B18)/3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D24" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A26" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1704,33 +1704,33 @@
   <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29" style="19" customWidth="1"/>
-    <col min="2" max="2" width="34.5" style="21" customWidth="1"/>
-    <col min="3" max="3" width="69.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="34.5703125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="69.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C4" s="24" t="s">
         <v>2</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C5" s="24" t="s">
         <v>3</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C6" s="24" t="s">
         <v>4</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C7" s="24" t="s">
         <v>5</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B8" s="21" t="s">
         <v>6</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C9" s="24" t="s">
         <v>20</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C10" s="24" t="s">
         <v>21</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C11" s="24" t="s">
         <v>22</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C12" s="24" t="s">
         <v>23</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C13" s="24" t="s">
         <v>24</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" s="22" t="s">
         <v>7</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C15" s="24" t="s">
         <v>25</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C16" s="24" t="s">
         <v>26</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C17" s="24" t="s">
         <v>27</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C18" s="24" t="s">
         <v>28</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C19" s="24" t="s">
         <v>29</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C20" s="24" t="s">
         <v>30</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C21" s="24" t="s">
         <v>31</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B22" s="22" t="s">
         <v>8</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C23" s="24" t="s">
         <v>32</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C24" s="24" t="s">
         <v>33</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C25" s="24" t="s">
         <v>34</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C26" s="24" t="s">
         <v>35</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
         <v>9</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B28" s="22" t="s">
         <v>10</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C29" s="24" t="s">
         <v>36</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C30" s="24" t="s">
         <v>37</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C31" s="24" t="s">
         <v>38</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C32" s="24" t="s">
         <v>39</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C33" s="24" t="s">
         <v>40</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C34" s="24" t="s">
         <v>41</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B35" s="22" t="s">
         <v>11</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C36" s="24" t="s">
         <v>42</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C37" s="24" t="s">
         <v>43</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C38" s="24" t="s">
         <v>44</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C39" s="24" t="s">
         <v>45</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C40" s="24" t="s">
         <v>46</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C41" s="24" t="s">
         <v>47</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B42" s="22" t="s">
         <v>12</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C43" s="24" t="s">
         <v>48</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C44" s="24" t="s">
         <v>49</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C45" s="24" t="s">
         <v>50</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C46" s="24" t="s">
         <v>51</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B47" s="22" t="s">
         <v>13</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C48" s="24" t="s">
         <v>52</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C49" s="24" t="s">
         <v>53</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C50" s="24" t="s">
         <v>54</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C51" s="24" t="s">
         <v>55</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="20" t="s">
         <v>14</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B53" s="22" t="s">
         <v>15</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C54" s="24" t="s">
         <v>56</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C55" s="24" t="s">
         <v>57</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C56" s="24" t="s">
         <v>58</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C57" s="24" t="s">
         <v>59</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C58" s="24" t="s">
         <v>60</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B59" s="22" t="s">
         <v>16</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C60" s="24" t="s">
         <v>61</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C61" s="24" t="s">
         <v>62</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C62" s="24" t="s">
         <v>63</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C63" s="24" t="s">
         <v>64</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C64" s="24" t="s">
         <v>65</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C65" s="24" t="s">
         <v>66</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C66" s="24" t="s">
         <v>67</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C67" s="24" t="s">
         <v>68</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C68" s="24" t="s">
         <v>69</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B69" s="22" t="s">
         <v>17</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C70" s="24" t="s">
         <v>70</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C71" s="24" t="s">
         <v>71</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C72" s="24" t="s">
         <v>72</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C73" s="24" t="s">
         <v>73</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B74" s="22" t="s">
         <v>18</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C75" s="24" t="s">
         <v>74</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C76" s="24" t="s">
         <v>75</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C77" s="24" t="s">
         <v>76</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B78" s="22" t="s">
         <v>19</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C79" s="24" t="s">
         <v>77</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C80" s="24" t="s">
         <v>78</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C81" s="24" t="s">
         <v>79</v>
       </c>
@@ -2681,28 +2681,28 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="12.5" style="3"/>
+    <col min="1" max="1" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="12.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>83</v>
       </c>
@@ -2713,15 +2713,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2730,7 +2721,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EF07142713CD6D4C83CBD8BC01D705B5" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="32aeae619b2d68ad0a0a617232c5ed1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="fdf91ed2-bd70-42ba-ab71-fba0383985f7" xmlns:ns4="f0622a8f-13ca-4d7c-a754-eaa399ac8b4a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3241b21036c9de17defa365b42b3bf51" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2970,17 +2961,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D59C97D4-D35A-4BE7-99D7-230B389AC139}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F35C236B-8AE1-436F-B1E2-ED8D2060C8FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2988,7 +2978,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EDD4A3B-2670-4E44-82A3-4A8CB7637D80}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3006,4 +2996,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D59C97D4-D35A-4BE7-99D7-230B389AC139}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>